<commit_message>
Improve accuracy of daily driver reports and report generation times
Refactor daily report generation logic, update PDF creation timestamps, and modify JSON report structures in exports/ and static/exports/.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: b83b866c-5b8f-4d82-9fde-612e7a355315
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/f2699832-8135-4557-9ec0-8d4d723b9ba2/ad452c28-271a-45ee-b3da-7b299a605765.jpg
</commit_message>
<xml_diff>
--- a/exports/daily_reports/2025-05-15_DailyDriverReport.xlsx
+++ b/exports/daily_reports/2025-05-15_DailyDriverReport.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,14 +425,89 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>employee_id</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>asset</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>arrival</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>division</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>job_title</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Roger Doddy</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>DODROG</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>PT-07S</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>04:45 AM</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>TEXDIST</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Select Maintenance Employee</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>